<commit_message>
fixed spelling error in spreadsheet
</commit_message>
<xml_diff>
--- a/Source/Workflows.Test/Data/TransferTimeSeriesTemplate.xlsx
+++ b/Source/Workflows.Test/Data/TransferTimeSeriesTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAM\source\repos\DHI\DomainServicesCourse\Source\Workflows.Test\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED20C4DA-48F7-4616-982A-AFAB25A671D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935A65DD-705C-48A4-B4E1-1C05E6D1105C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MIKE11" sheetId="1" r:id="rId1"/>
@@ -63,9 +63,6 @@
     <t>m</t>
   </si>
   <si>
-    <t>Offsett</t>
-  </si>
-  <si>
     <t>CALI-HD.res11/Reach;Water Level;CALI;0</t>
   </si>
   <si>
@@ -78,10 +75,13 @@
     <t>[root]\Current\CALI-HD.res11</t>
   </si>
   <si>
-    <t>CaliSimulationResults/water-level-reach-0</t>
-  </si>
-  <si>
     <t>apiKey=90892a37-668b-4be8-bd7c-cc33eea4eda1;projectId=536f2d5c-988f-423d-84c4-f1a2a0e07afe</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
+    <t>CaliSimulationResults/water-level-reach-0-[id]</t>
   </si>
 </sst>
 </file>
@@ -407,8 +407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,7 +444,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
@@ -461,19 +461,19 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -482,7 +482,7 @@
         <v>9</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J2" t="s">
         <v>11</v>

</xml_diff>